<commit_message>
modified report html and css
</commit_message>
<xml_diff>
--- a/upload/Template-Cart.xlsx
+++ b/upload/Template-Cart.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
   <si>
     <t>No</t>
   </si>
@@ -52,13 +52,19 @@
     <t>GSMF-GTZ-5S</t>
   </si>
   <si>
-    <t>12-100020-00000</t>
-  </si>
-  <si>
-    <t>12-100020-FLAP</t>
-  </si>
-  <si>
-    <t>12-50012-00000</t>
+    <t>FP-W0045-F1Z-2700</t>
+  </si>
+  <si>
+    <t>FP-43125-KGA-2700</t>
+  </si>
+  <si>
+    <t>FP-43120-362-2700</t>
+  </si>
+  <si>
+    <t>FP-54410-THU-2700</t>
+  </si>
+  <si>
+    <t>FP-F533A-RXK-2700</t>
   </si>
 </sst>
 </file>
@@ -421,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -471,7 +477,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="9">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>4</v>
@@ -485,9 +491,37 @@
         <v>12</v>
       </c>
       <c r="C4" s="9">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="9">
+        <v>20</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="9">
+        <v>20</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>